<commit_message>
Automatic Selection of the grid File
</commit_message>
<xml_diff>
--- a/FolderOverview.xlsx
+++ b/FolderOverview.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\PycharmProjects\TecplotPropeller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E1416C5-A499-46B3-9868-D0767696B3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B092AFB0-1D95-4082-A795-5B69A293C939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{1FB1D09D-BF53-47CB-AC77-59B83470E293}"/>
+    <workbookView xWindow="-48" yWindow="-48" windowWidth="23136" windowHeight="12456" activeTab="1" xr2:uid="{1FB1D09D-BF53-47CB-AC77-59B83470E293}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
   <si>
     <t>Folder Number</t>
   </si>
@@ -108,20 +109,6 @@
   </si>
   <si>
     <r>
-      <t>masscaught</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>()</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>collection</t>
     </r>
     <r>
@@ -214,12 +201,112 @@
   <si>
     <t>25_RWHeatFlow</t>
   </si>
+  <si>
+    <r>
+      <t>mainRun</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <t>38_RWHeatFlow</t>
+  </si>
+  <si>
+    <t>35_Collection</t>
+  </si>
+  <si>
+    <r>
+      <t>Collection efficiency-Droplet'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Droplet LWC (kg/m^3)</t>
+    </r>
+  </si>
+  <si>
+    <t>Flight Part 1:</t>
+  </si>
+  <si>
+    <t>Airspeed</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Airspeed </t>
+  </si>
+  <si>
+    <t>Carbon firbe resistance:</t>
+  </si>
+  <si>
+    <t>Zone width [mm]</t>
+  </si>
+  <si>
+    <t>Zone length [mm]</t>
+  </si>
+  <si>
+    <t>Numberÿ of carbonÿ layers 100g/m2</t>
+  </si>
+  <si>
+    <t>unlaminated</t>
+  </si>
+  <si>
+    <t>laminated</t>
+  </si>
+  <si>
+    <t>Gramm/meter</t>
+  </si>
+  <si>
+    <t>Resistance/meter</t>
+  </si>
+  <si>
+    <t>Diff to mean</t>
+  </si>
+  <si>
+    <t>relative dif</t>
+  </si>
+  <si>
+    <t>Tex</t>
+  </si>
+  <si>
+    <t>Resistance*Tex</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,6 +329,12 @@
     <font>
       <sz val="9.8000000000000007"/>
       <color rgb="FFFFC66D"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFCC7832"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
@@ -289,6 +382,913 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$G$33:$G$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>25.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34.74</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$H$33:$H$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>682.56000000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>912.48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1369.92</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4768-47AB-A8A0-10F56B61EFBE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1093086256"/>
+        <c:axId val="1093086672"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1093086256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1093086672"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1093086672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1093086256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62BE4A87-3025-4D22-916B-8988AD1636A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -590,13 +1590,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{807D7481-6AB9-431B-A309-52B3EF598035}">
   <dimension ref="A5:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="13.47265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.15625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
   </cols>
@@ -688,7 +1688,7 @@
         <v>8</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -756,10 +1756,10 @@
         <v>21</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
@@ -768,7 +1768,7 @@
         <v>19</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -788,7 +1788,7 @@
         <v>19</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -796,10 +1796,10 @@
         <v>23</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
@@ -808,7 +1808,7 @@
         <v>19</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -816,10 +1816,10 @@
         <v>24</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
@@ -828,7 +1828,7 @@
         <v>19</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -836,10 +1836,10 @@
         <v>25</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D30" t="s">
         <v>12</v>
@@ -848,7 +1848,7 @@
         <v>19</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -861,32 +1861,32 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:6">
       <c r="A37">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>33</v>
       </c>
@@ -902,8 +1902,11 @@
       <c r="E38" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>34</v>
       </c>
@@ -919,48 +1922,81 @@
       <c r="E39" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>35</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="B40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:6">
       <c r="A42">
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:6">
       <c r="A43">
         <v>38</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="B43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44">
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:6">
       <c r="A45">
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:6">
       <c r="A46">
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:6">
       <c r="A47">
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:6">
       <c r="A48">
         <v>43</v>
       </c>
@@ -1211,4 +2247,1092 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA68D4E-E5C0-47AF-A233-8314B3239060}">
+  <dimension ref="A2:N87"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="12" max="12" width="11.68359375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <f>A2*9.81</f>
+        <v>215.82000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3">
+        <v>1.2250000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D4">
+        <f>B2*2/A3/A4/B5</f>
+        <v>0.19149955634427684</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <f>A5^2</f>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="C8">
+        <f>0.0243</f>
+        <v>2.4299999999999999E-2</v>
+      </c>
+      <c r="D8">
+        <v>6.2E-2</v>
+      </c>
+      <c r="E8">
+        <f>C8+D8*D4</f>
+        <v>3.6172972493345161E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="F10">
+        <f>E8*0.5*B5*A3</f>
+        <v>35.449513043478255</v>
+      </c>
+      <c r="I10">
+        <f>F10*A5</f>
+        <v>1417.9805217391302</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="I12">
+        <f>I10/0.6</f>
+        <v>2363.300869565217</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="B18">
+        <f>3300/48</f>
+        <v>68.75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="B28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28">
+        <v>29.98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29">
+        <v>5.98</v>
+      </c>
+      <c r="D29">
+        <f>C29*48</f>
+        <v>287.04000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30">
+        <v>37.82</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ref="D30:D31" si="0">C30*48</f>
+        <v>1815.3600000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="B31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31">
+        <v>19.010000000000002</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>912.48</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8">
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33">
+        <v>34.74</v>
+      </c>
+      <c r="G33">
+        <v>25.03</v>
+      </c>
+      <c r="H33">
+        <v>682.56000000000006</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8">
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34">
+        <v>9.93</v>
+      </c>
+      <c r="D34">
+        <f>C34*48</f>
+        <v>476.64</v>
+      </c>
+      <c r="G34">
+        <v>29.98</v>
+      </c>
+      <c r="H34">
+        <v>912.48</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35">
+        <v>51.75</v>
+      </c>
+      <c r="D35">
+        <f t="shared" ref="D35:D36" si="1">C35*48</f>
+        <v>2484</v>
+      </c>
+      <c r="G35">
+        <v>34.74</v>
+      </c>
+      <c r="H35">
+        <v>1369.92</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36">
+        <v>28.54</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>1369.92</v>
+      </c>
+      <c r="G36">
+        <v>25.03</v>
+      </c>
+      <c r="H36">
+        <v>682.56000000000006</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8">
+      <c r="B39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39">
+        <v>25.03</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="B40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="D40">
+        <f>C40*48</f>
+        <v>213.12</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8">
+      <c r="B41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <v>26.71</v>
+      </c>
+      <c r="D41">
+        <f t="shared" ref="D41:D42" si="2">C41*48</f>
+        <v>1282.08</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8">
+      <c r="B42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <v>14.22</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="2"/>
+        <v>682.56000000000006</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="B52">
+        <v>38000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="B55" t="s">
+        <v>44</v>
+      </c>
+      <c r="C55" t="s">
+        <v>45</v>
+      </c>
+      <c r="D55" t="s">
+        <v>46</v>
+      </c>
+      <c r="F55" t="s">
+        <v>47</v>
+      </c>
+      <c r="G55" t="s">
+        <v>48</v>
+      </c>
+      <c r="H55" t="s">
+        <v>49</v>
+      </c>
+      <c r="I55" t="s">
+        <v>50</v>
+      </c>
+      <c r="K55" t="s">
+        <v>51</v>
+      </c>
+      <c r="L55" t="s">
+        <v>52</v>
+      </c>
+      <c r="M55" t="s">
+        <v>53</v>
+      </c>
+      <c r="N55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
+      <c r="B56">
+        <v>20</v>
+      </c>
+      <c r="C56">
+        <v>630</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>100</v>
+      </c>
+      <c r="F56">
+        <v>9.4</v>
+      </c>
+      <c r="G56">
+        <v>7.8</v>
+      </c>
+      <c r="H56">
+        <f>E56*D56*B56/1000</f>
+        <v>2</v>
+      </c>
+      <c r="I56">
+        <f>G56/C56*1000</f>
+        <v>12.380952380952381</v>
+      </c>
+      <c r="J56">
+        <f>I56*H56</f>
+        <v>24.761904761904763</v>
+      </c>
+      <c r="K56">
+        <f>ABS(J56-$J$71)</f>
+        <v>4</v>
+      </c>
+      <c r="L56">
+        <f>K56/$J$71</f>
+        <v>0.13907284768211919</v>
+      </c>
+      <c r="M56">
+        <f>H56*1000</f>
+        <v>2000</v>
+      </c>
+      <c r="N56">
+        <f>I56*M56</f>
+        <v>24761.904761904763</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="B57">
+        <v>20</v>
+      </c>
+      <c r="C57">
+        <v>630</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>100</v>
+      </c>
+      <c r="F57">
+        <v>4</v>
+      </c>
+      <c r="G57">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H57">
+        <f t="shared" ref="H57:H70" si="3">E57*D57*B57/1000</f>
+        <v>4</v>
+      </c>
+      <c r="I57">
+        <f t="shared" ref="I57:I70" si="4">G57/C57*1000</f>
+        <v>6.5079365079365079</v>
+      </c>
+      <c r="J57">
+        <f t="shared" ref="J57:J70" si="5">I57*H57</f>
+        <v>26.031746031746032</v>
+      </c>
+      <c r="K57">
+        <f t="shared" ref="K57:K70" si="6">ABS(J57-$J$71)</f>
+        <v>2.7301587301587311</v>
+      </c>
+      <c r="L57">
+        <f t="shared" ref="L57:L70" si="7">K57/$J$71</f>
+        <v>9.4922737306843294E-2</v>
+      </c>
+      <c r="M57">
+        <f t="shared" ref="M57:M70" si="8">H57*1000</f>
+        <v>4000</v>
+      </c>
+      <c r="N57">
+        <f t="shared" ref="N57:N70" si="9">I57*M57</f>
+        <v>26031.746031746032</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
+      <c r="B58">
+        <v>20</v>
+      </c>
+      <c r="C58">
+        <v>630</v>
+      </c>
+      <c r="D58">
+        <v>3</v>
+      </c>
+      <c r="E58">
+        <v>100</v>
+      </c>
+      <c r="F58">
+        <v>2.9</v>
+      </c>
+      <c r="G58">
+        <v>2.8</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="4"/>
+        <v>4.4444444444444446</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="5"/>
+        <v>26.666666666666668</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="6"/>
+        <v>2.0952380952380949</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="7"/>
+        <v>7.2847682119205281E-2</v>
+      </c>
+      <c r="M58">
+        <f t="shared" si="8"/>
+        <v>6000</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="9"/>
+        <v>26666.666666666668</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
+      <c r="B59">
+        <v>20</v>
+      </c>
+      <c r="C59">
+        <v>630</v>
+      </c>
+      <c r="D59">
+        <v>4</v>
+      </c>
+      <c r="E59">
+        <v>100</v>
+      </c>
+      <c r="F59">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G59">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="4"/>
+        <v>3.6507936507936507</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="5"/>
+        <v>29.206349206349206</v>
+      </c>
+      <c r="K59">
+        <f t="shared" si="6"/>
+        <v>0.44444444444444287</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="7"/>
+        <v>1.5452538631346524E-2</v>
+      </c>
+      <c r="M59">
+        <f t="shared" si="8"/>
+        <v>8000</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="9"/>
+        <v>29206.349206349205</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="B60">
+        <v>20</v>
+      </c>
+      <c r="C60">
+        <v>630</v>
+      </c>
+      <c r="D60">
+        <v>5</v>
+      </c>
+      <c r="E60">
+        <v>100</v>
+      </c>
+      <c r="F60">
+        <v>1.8</v>
+      </c>
+      <c r="G60">
+        <v>2</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="4"/>
+        <v>3.1746031746031744</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="5"/>
+        <v>31.746031746031743</v>
+      </c>
+      <c r="K60">
+        <f t="shared" si="6"/>
+        <v>2.9841269841269806</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="7"/>
+        <v>0.10375275938189833</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="8"/>
+        <v>10000</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="9"/>
+        <v>31746.031746031746</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="B61">
+        <v>40</v>
+      </c>
+      <c r="C61">
+        <v>630</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>100</v>
+      </c>
+      <c r="F61">
+        <v>4.3</v>
+      </c>
+      <c r="G61">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="4"/>
+        <v>7.3015873015873014</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="5"/>
+        <v>29.206349206349206</v>
+      </c>
+      <c r="K61">
+        <f t="shared" si="6"/>
+        <v>0.44444444444444287</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="7"/>
+        <v>1.5452538631346524E-2</v>
+      </c>
+      <c r="M61">
+        <f t="shared" si="8"/>
+        <v>4000</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="9"/>
+        <v>29206.349206349205</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="B62">
+        <v>40</v>
+      </c>
+      <c r="C62">
+        <v>630</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62">
+        <v>100</v>
+      </c>
+      <c r="F62">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G62">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="4"/>
+        <v>3.6507936507936507</v>
+      </c>
+      <c r="J62">
+        <f t="shared" si="5"/>
+        <v>29.206349206349206</v>
+      </c>
+      <c r="K62">
+        <f t="shared" si="6"/>
+        <v>0.44444444444444287</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="7"/>
+        <v>1.5452538631346524E-2</v>
+      </c>
+      <c r="M62">
+        <f t="shared" si="8"/>
+        <v>8000</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="9"/>
+        <v>29206.349206349205</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
+      <c r="B63">
+        <v>40</v>
+      </c>
+      <c r="C63">
+        <v>630</v>
+      </c>
+      <c r="D63">
+        <v>3</v>
+      </c>
+      <c r="E63">
+        <v>100</v>
+      </c>
+      <c r="F63">
+        <v>1.6</v>
+      </c>
+      <c r="G63">
+        <v>1.6</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="4"/>
+        <v>2.5396825396825395</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="5"/>
+        <v>30.476190476190474</v>
+      </c>
+      <c r="K63">
+        <f t="shared" si="6"/>
+        <v>1.7142857142857117</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="7"/>
+        <v>5.9602649006622425E-2</v>
+      </c>
+      <c r="M63">
+        <f t="shared" si="8"/>
+        <v>12000</v>
+      </c>
+      <c r="N63">
+        <f t="shared" si="9"/>
+        <v>30476.190476190473</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
+      <c r="B64">
+        <v>40</v>
+      </c>
+      <c r="C64">
+        <v>630</v>
+      </c>
+      <c r="D64">
+        <v>4</v>
+      </c>
+      <c r="E64">
+        <v>100</v>
+      </c>
+      <c r="F64">
+        <v>1.2</v>
+      </c>
+      <c r="G64">
+        <v>1.2</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="4"/>
+        <v>1.9047619047619047</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="5"/>
+        <v>30.476190476190474</v>
+      </c>
+      <c r="K64">
+        <f t="shared" si="6"/>
+        <v>1.7142857142857117</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="7"/>
+        <v>5.9602649006622425E-2</v>
+      </c>
+      <c r="M64">
+        <f t="shared" si="8"/>
+        <v>16000</v>
+      </c>
+      <c r="N64">
+        <f t="shared" si="9"/>
+        <v>30476.190476190473</v>
+      </c>
+    </row>
+    <row r="65" spans="2:14">
+      <c r="B65">
+        <v>60</v>
+      </c>
+      <c r="C65">
+        <v>630</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>100</v>
+      </c>
+      <c r="F65">
+        <v>2.9</v>
+      </c>
+      <c r="G65">
+        <v>2.8</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="4"/>
+        <v>4.4444444444444446</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="5"/>
+        <v>26.666666666666668</v>
+      </c>
+      <c r="K65">
+        <f t="shared" si="6"/>
+        <v>2.0952380952380949</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="7"/>
+        <v>7.2847682119205281E-2</v>
+      </c>
+      <c r="M65">
+        <f t="shared" si="8"/>
+        <v>6000</v>
+      </c>
+      <c r="N65">
+        <f t="shared" si="9"/>
+        <v>26666.666666666668</v>
+      </c>
+    </row>
+    <row r="66" spans="2:14">
+      <c r="B66">
+        <v>60</v>
+      </c>
+      <c r="C66">
+        <v>630</v>
+      </c>
+      <c r="D66">
+        <v>2</v>
+      </c>
+      <c r="E66">
+        <v>100</v>
+      </c>
+      <c r="F66">
+        <v>1.8</v>
+      </c>
+      <c r="G66">
+        <v>1.5</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="4"/>
+        <v>2.3809523809523814</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="5"/>
+        <v>28.571428571428577</v>
+      </c>
+      <c r="K66">
+        <f t="shared" si="6"/>
+        <v>0.19047619047618625</v>
+      </c>
+      <c r="L66">
+        <f t="shared" si="7"/>
+        <v>6.6225165562912433E-3</v>
+      </c>
+      <c r="M66">
+        <f t="shared" si="8"/>
+        <v>12000</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="9"/>
+        <v>28571.428571428576</v>
+      </c>
+    </row>
+    <row r="67" spans="2:14">
+      <c r="B67">
+        <v>60</v>
+      </c>
+      <c r="C67">
+        <v>630</v>
+      </c>
+      <c r="D67">
+        <v>3</v>
+      </c>
+      <c r="E67">
+        <v>100</v>
+      </c>
+      <c r="F67">
+        <v>1.2</v>
+      </c>
+      <c r="G67">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="4"/>
+        <v>1.7460317460317463</v>
+      </c>
+      <c r="J67">
+        <f t="shared" si="5"/>
+        <v>31.428571428571434</v>
+      </c>
+      <c r="K67">
+        <f t="shared" si="6"/>
+        <v>2.6666666666666714</v>
+      </c>
+      <c r="L67">
+        <f t="shared" si="7"/>
+        <v>9.2715231788079638E-2</v>
+      </c>
+      <c r="M67">
+        <f t="shared" si="8"/>
+        <v>18000</v>
+      </c>
+      <c r="N67">
+        <f t="shared" si="9"/>
+        <v>31428.571428571431</v>
+      </c>
+    </row>
+    <row r="68" spans="2:14">
+      <c r="B68">
+        <v>80</v>
+      </c>
+      <c r="C68">
+        <v>630</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>100</v>
+      </c>
+      <c r="F68">
+        <v>2.6</v>
+      </c>
+      <c r="G68">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="4"/>
+        <v>3.4920634920634925</v>
+      </c>
+      <c r="J68">
+        <f t="shared" si="5"/>
+        <v>27.93650793650794</v>
+      </c>
+      <c r="K68">
+        <f t="shared" si="6"/>
+        <v>0.82539682539682246</v>
+      </c>
+      <c r="L68">
+        <f t="shared" si="7"/>
+        <v>2.8697571743929257E-2</v>
+      </c>
+      <c r="M68">
+        <f t="shared" si="8"/>
+        <v>8000</v>
+      </c>
+      <c r="N68">
+        <f t="shared" si="9"/>
+        <v>27936.50793650794</v>
+      </c>
+    </row>
+    <row r="69" spans="2:14">
+      <c r="B69">
+        <v>80</v>
+      </c>
+      <c r="C69">
+        <v>630</v>
+      </c>
+      <c r="D69">
+        <v>2</v>
+      </c>
+      <c r="E69">
+        <v>100</v>
+      </c>
+      <c r="F69">
+        <v>1.6</v>
+      </c>
+      <c r="G69">
+        <v>1.2</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="4"/>
+        <v>1.9047619047619047</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="5"/>
+        <v>30.476190476190474</v>
+      </c>
+      <c r="K69">
+        <f t="shared" si="6"/>
+        <v>1.7142857142857117</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="7"/>
+        <v>5.9602649006622425E-2</v>
+      </c>
+      <c r="M69">
+        <f t="shared" si="8"/>
+        <v>16000</v>
+      </c>
+      <c r="N69">
+        <f t="shared" si="9"/>
+        <v>30476.190476190473</v>
+      </c>
+    </row>
+    <row r="70" spans="2:14">
+      <c r="B70">
+        <v>100</v>
+      </c>
+      <c r="C70">
+        <v>630</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>100</v>
+      </c>
+      <c r="F70">
+        <v>2</v>
+      </c>
+      <c r="G70">
+        <v>1.8</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="4"/>
+        <v>2.8571428571428572</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="5"/>
+        <v>28.571428571428573</v>
+      </c>
+      <c r="K70">
+        <f t="shared" si="6"/>
+        <v>0.1904761904761898</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="7"/>
+        <v>6.6225165562913673E-3</v>
+      </c>
+      <c r="M70">
+        <f t="shared" si="8"/>
+        <v>10000</v>
+      </c>
+      <c r="N70">
+        <f t="shared" si="9"/>
+        <v>28571.428571428572</v>
+      </c>
+    </row>
+    <row r="71" spans="2:14">
+      <c r="J71">
+        <f>AVERAGE(J56:J70)</f>
+        <v>28.761904761904763</v>
+      </c>
+    </row>
+    <row r="76" spans="2:14">
+      <c r="B76">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="77" spans="2:14">
+      <c r="B77">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="78" spans="2:14">
+      <c r="B78">
+        <f>B77/B76</f>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="79" spans="2:14">
+      <c r="B79">
+        <f>B76/B78</f>
+        <v>3.84</v>
+      </c>
+    </row>
+    <row r="80" spans="2:14">
+      <c r="B80">
+        <f>B76/B78*2</f>
+        <v>7.68</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3">
+      <c r="B81">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3">
+      <c r="B82">
+        <f>B80*1000/B81</f>
+        <v>30.72</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3">
+      <c r="B83">
+        <f>N70/B82</f>
+        <v>930.05952380952385</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3">
+      <c r="B84">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3">
+      <c r="B85">
+        <f>B83/1000/B84</f>
+        <v>5.4709383753501401E-4</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3">
+      <c r="B86">
+        <v>2.5999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3">
+      <c r="B87">
+        <f>B85/B86</f>
+        <v>2.1042070674423616</v>
+      </c>
+      <c r="C87" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cleanup of the scripts Remove unneccesary functions
</commit_message>
<xml_diff>
--- a/FolderOverview.xlsx
+++ b/FolderOverview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\PycharmProjects\TecplotPropeller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B8086C-D98E-4D74-AE99-8421F3ABA4BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF3FC84-5BDF-4F6C-B25B-BF4BFF24F0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48" yWindow="-48" windowWidth="23136" windowHeight="12456" activeTab="1" xr2:uid="{1FB1D09D-BF53-47CB-AC77-59B83470E293}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{1FB1D09D-BF53-47CB-AC77-59B83470E293}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4455,7 +4455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA68D4E-E5C0-47AF-A233-8314B3239060}">
   <dimension ref="A2:X87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
       <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
@@ -4715,7 +4715,7 @@
         <v>1.1254999999999999</v>
       </c>
       <c r="U45">
-        <f t="shared" ref="U44:V53" si="3">T45*1000</f>
+        <f t="shared" ref="U45:U53" si="3">T45*1000</f>
         <v>1125.5</v>
       </c>
       <c r="V45">

</xml_diff>